<commit_message>
Eliminación de Tab de configuración, se realizan ajustes en los módulos reqeuridos y se realizan modificaciones varias de optimización y mejora de código.
</commit_message>
<xml_diff>
--- a/plantilla_importacion_servicios.xlsx
+++ b/plantilla_importacion_servicios.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,27 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004F81BD"/>
-        <bgColor rgb="004F81BD"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -69,13 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,54 +432,44 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="11" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>id_carpeta</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>id_servicio</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>id_predio</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>id_tercero_cliente</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>periodo_inicio_cobro</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>lectura_anterior</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>lectura_actual</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>valor_unitario</t>
         </is>

</xml_diff>